<commit_message>
Deploying to main from @ INTI-CMNB/kibot_variants_arduprog@b0b88aaf704b27ef21d94235e3ab51ab837c69e1 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/t1-bom.xlsx
+++ b/BoM/Positional/t1-bom.xlsx
@@ -187,7 +187,7 @@
     <t>270.0000</t>
   </si>
   <si>
-    <t>Net-(U1-UCAP),Earth</t>
+    <t>Earth,Net-(U1-UCAP)</t>
   </si>
   <si>
     <t>3</t>
@@ -283,7 +283,7 @@
     <t>-74.9500</t>
   </si>
   <si>
-    <t>/RXLED,Net-(D2-A)</t>
+    <t>Net-(D2-A),/RXLED</t>
   </si>
   <si>
     <t>6</t>
@@ -319,7 +319,7 @@
     <t>14.0000</t>
   </si>
   <si>
-    <t>,+5V,GND</t>
+    <t>,GND,+5V</t>
   </si>
   <si>
     <t>7</t>
@@ -361,7 +361,7 @@
     <t>6.7800</t>
   </si>
   <si>
-    <t>/MISO2,/MOSI2,/SCK2,+5V,GND,/RESET2</t>
+    <t>/SCK2,/MOSI2,/RESET2,/MISO2,GND,+5V</t>
   </si>
   <si>
     <t>8</t>
@@ -397,7 +397,7 @@
     <t>11.8600</t>
   </si>
   <si>
-    <t>Net-(J3-Pin_5),Net-(J3-Pin_1),Net-(J3-Pin_4),Net-(J3-Pin_2),Net-(J3-Pin_3)</t>
+    <t>Net-(J3-Pin_5),Net-(J3-Pin_3),Net-(J3-Pin_1),Net-(J3-Pin_2),Net-(J3-Pin_4)</t>
   </si>
   <si>
     <t>9</t>
@@ -427,7 +427,7 @@
     <t>14.4000</t>
   </si>
   <si>
-    <t>Net-(J6-Pin_2),Net-(J6-Pin_5),Net-(J6-Pin_3),Net-(J6-Pin_1),Net-(J6-Pin_4),Net-(J6-Pin_6)</t>
+    <t>Net-(J6-Pin_6),Net-(J6-Pin_5),Net-(J6-Pin_4),Net-(J6-Pin_1),Net-(J6-Pin_2),Net-(J6-Pin_3)</t>
   </si>
   <si>
     <t>10</t>
@@ -547,7 +547,7 @@
     <t>10.1000</t>
   </si>
   <si>
-    <t>Net-(J4-Pin_4),Net-(J3-Pin_1),Net-(U1-D+),Net-(J3-Pin_5),/MISO2,/MOSI2,Net-(U1-UCAP),Net-(J6-Pin_5),Net-(J4-Pin_1),Net-(U1-D-),Net-(J6-Pin_4),+5V,Net-(J3-Pin_2),unconnected-(U1-PB0-Pad14),/RESET2,VBUS,Net-(J6-Pin_6),Net-(J4-Pin_3),/RXLED,Earth,/DTR,GND,/TXLED,Net-(J3-Pin_3),Net-(J6-Pin_2),Net-(U1-XTAL1),Net-(J6-Pin_3),/SCK2,Net-(J3-Pin_4),Net-(J4-Pin_2),Net-(U1-PC0{slash}XTAL2)</t>
+    <t>/RESET2,Net-(J4-Pin_1),Net-(U1-XTAL1),Net-(J4-Pin_2),/MISO2,/MOSI2,Net-(J3-Pin_3),Net-(U1-UCAP),/DTR,VBUS,Net-(J4-Pin_3),Net-(J6-Pin_3),Net-(J3-Pin_4),Net-(U1-PC0{slash}XTAL2),+5V,/SCK2,Net-(J3-Pin_5),Net-(J6-Pin_4),Net-(U1-D+),Net-(J4-Pin_4),Net-(J3-Pin_2),Net-(U1-D-),GND,unconnected-(U1-PB0-Pad14),Net-(J6-Pin_2),Net-(J6-Pin_6),Net-(J6-Pin_5),Net-(J3-Pin_1),/RXLED,/TXLED,Earth</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -625,7 +625,7 @@
     <t>no</t>
   </si>
   <si>
-    <t>Net-(U1-XTAL1),GND</t>
+    <t>GND,Net-(U1-XTAL1)</t>
   </si>
   <si>
     <t>Resettable fuse, polymeric positive temperature coefficient</t>
@@ -694,7 +694,7 @@
     <t>-95.2500</t>
   </si>
   <si>
-    <t>Net-(J4-Pin_3),Net-(J4-Pin_4),Net-(J4-Pin_2),Net-(J4-Pin_1)</t>
+    <t>Net-(J4-Pin_4),Net-(J4-Pin_2),Net-(J4-Pin_1),Net-(J4-Pin_3)</t>
   </si>
   <si>
     <t>USB Type B connector</t>
@@ -727,7 +727,7 @@
     <t>16.0000</t>
   </si>
   <si>
-    <t>Net-(J2-VBUS),Net-(J2-D-),Net-(J2-D+),Earth,Net-(J2-Shield)</t>
+    <t>Net-(J2-VBUS),Earth,Net-(J2-Shield),Net-(J2-D+),Net-(J2-D-)</t>
   </si>
   <si>
     <t>R1 R2</t>
@@ -757,7 +757,7 @@
     <t>-75.8780</t>
   </si>
   <si>
-    <t>Net-(U1-XTAL1),Net-(U1-PC0{slash}XTAL2)</t>
+    <t>Net-(U1-PC0{slash}XTAL2),Net-(U1-XTAL1)</t>
   </si>
   <si>
     <t>Voltage dependent resistor</t>
@@ -787,7 +787,7 @@
     <t>0.9500</t>
   </si>
   <si>
-    <t>Net-(J2-Shield),Net-(J2-D+)</t>
+    <t>Net-(J2-D+),Net-(J2-Shield)</t>
   </si>
   <si>
     <t>Two pin crystal</t>

</xml_diff>